<commit_message>
add cap statements for all actors
</commit_message>
<xml_diff>
--- a/source/resources/source-data/alert-sender.xlsx
+++ b/source/resources/source-data/alert-sender.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ERICS-AIR-2\ehaas\Documents\FHIR\Davinci-Alerts\source\resources\source-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6A33B8B-BCC2-475B-885E-4DDE89402562}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2435F8AC-7164-4008-A59F-E23D5246E6C3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17535" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,13 @@
     <sheet name="resources" sheetId="4" r:id="rId4"/>
     <sheet name="ops" sheetId="5" r:id="rId5"/>
     <sheet name="interactions" sheetId="6" r:id="rId6"/>
-    <sheet name="sps" sheetId="7" r:id="rId7"/>
-    <sheet name="sp_combos" sheetId="8" r:id="rId8"/>
+    <sheet name="rest_interactions" sheetId="11" r:id="rId7"/>
+    <sheet name="sps" sheetId="7" r:id="rId8"/>
+    <sheet name="sp_combos" sheetId="8" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">sp_combos!$B$1:$B$81</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">sps!$A$1:$AB$92</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">sp_combos!$B$1:$B$81</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">sps!$A$1:$AB$92</definedName>
   </definedNames>
   <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
@@ -72,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="118">
   <si>
     <t>Element</t>
   </si>
@@ -272,18 +273,6 @@
     <t>should_include</t>
   </si>
   <si>
-    <t>conf_AllergyIntolerance</t>
-  </si>
-  <si>
-    <t>conf_CarePlan</t>
-  </si>
-  <si>
-    <t>conf_CareTeam</t>
-  </si>
-  <si>
-    <t>conf_Condition</t>
-  </si>
-  <si>
     <t>conf_Device</t>
   </si>
   <si>
@@ -374,17 +363,10 @@
     <t>referencePolicy_conf</t>
   </si>
   <si>
-    <t>1. See the [General Security Considerations](security.html) section for requirements and recommendations.
-1. A server **SHALL** reject any unauthorized requests by returning an `HTTP 401` unauthorized response code.</t>
-  </si>
-  <si>
     <t>doc_DiagnosticReport</t>
   </si>
   <si>
     <t>alert-sender</t>
-  </si>
-  <si>
-    <t>This Section describes the expected capabilities of the Da Vinci Alert Sender actor which is responsibleresponsible for sending the alert, typically operated by the facility or organization where the event occurred. The complete list of FHIR profiles, RESTful operations, and search parameters supported by Da Vinci Alert Senders are defined.</t>
   </si>
   <si>
     <t>http://hl7.org/fhir/us/davinci-alerts/CapabilityStatement/hl7.fhir.us.davinci-alerts-0.0.0</t>
@@ -428,6 +410,32 @@
   </si>
   <si>
     <t xml:space="preserve"> US Core Implementation Guide STU 3</t>
+  </si>
+  <si>
+    <t>transaction</t>
+  </si>
+  <si>
+    <t>batch</t>
+  </si>
+  <si>
+    <t>search-system</t>
+  </si>
+  <si>
+    <t>history-system</t>
+  </si>
+  <si>
+    <t>doc</t>
+  </si>
+  <si>
+    <t>Whether as a direct push based transaction or via subscription notification, a common  `transaction`  type “Alert Bundle” is the FHIR object that is exchanged between the Da Vinci Alert Actors.</t>
+  </si>
+  <si>
+    <t>This Section describes the expected capabilities of the Da Vinci Alert Sender actor which is responsible for sending the alert, typically operated by the facility or organization where the event occurred. The complete list of FHIR profiles, RESTful operations, and search parameters supported by Da Vinci Alert Senders are defined.</t>
+  </si>
+  <si>
+    <t>1. For general security consideration refer to the [Security and Privacy Considerations](http://build.fhir.org/secpriv-module.html). 
+1. For security considerations specific to this guide refer to the  [Security](security.html) page for requirements and recommendations.
+1. A server **SHALL** reject any unauthorized requests by returning an `HTTP 401` unauthorized response code.</t>
   </si>
 </sst>
 </file>
@@ -896,8 +904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -919,7 +927,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="105" customHeight="1">
@@ -927,7 +935,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -935,7 +943,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -951,7 +959,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="103.5" customHeight="1">
@@ -959,7 +967,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>100</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -971,7 +979,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A70CC787-78D8-4AA0-BE43-37746049F77C}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -993,10 +1001,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>13</v>
@@ -1039,16 +1047,16 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B2" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="F2" s="1"/>
     </row>
@@ -1172,49 +1180,49 @@
         <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F1" t="s">
         <v>17</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="H1" t="s">
         <v>18</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="R1" t="s">
         <v>19</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="T1" s="4" t="s">
         <v>64</v>
@@ -1223,15 +1231,15 @@
         <v>65</v>
       </c>
       <c r="V1" s="4" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="W1" s="4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="15.75" thickTop="1">
       <c r="A2" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>13</v>
@@ -1245,7 +1253,7 @@
     </row>
     <row r="3" spans="1:23">
       <c r="A3" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>13</v>
@@ -1259,7 +1267,7 @@
     </row>
     <row r="4" spans="1:23">
       <c r="A4" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>13</v>
@@ -1293,7 +1301,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1336,43 +1344,42 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:Y10"/>
+  <dimension ref="A1:U10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="Y1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AA23" sqref="AA23"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15" style="1" customWidth="1"/>
-    <col min="7" max="7" width="58.28515625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="28.140625" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" customWidth="1"/>
+    <col min="3" max="3" width="58.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="28.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:21">
       <c r="A1" t="s">
         <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>71</v>
@@ -1404,54 +1411,42 @@
       <c r="Q1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" t="s">
         <v>81</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>82</v>
+        <v>105</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>83</v>
+        <v>106</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="V1" t="s">
-        <v>85</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21">
       <c r="A2" t="s">
         <v>25</v>
       </c>
       <c r="B2" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F2" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I2" s="1" t="s">
+      <c r="G2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" t="s">
         <v>28</v>
       </c>
       <c r="J2" t="s">
@@ -1481,38 +1476,23 @@
       <c r="R2" t="s">
         <v>28</v>
       </c>
-      <c r="S2" t="s">
-        <v>28</v>
-      </c>
-      <c r="T2" t="s">
-        <v>28</v>
-      </c>
-      <c r="U2" t="s">
-        <v>28</v>
-      </c>
-      <c r="V2" t="s">
-        <v>28</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25">
+      <c r="S2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
       <c r="A3" t="s">
         <v>26</v>
       </c>
       <c r="B3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="D3" t="s">
         <v>13</v>
       </c>
@@ -1522,6 +1502,9 @@
       <c r="F3" t="s">
         <v>13</v>
       </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
       <c r="H3" t="s">
         <v>13</v>
       </c>
@@ -1555,38 +1538,23 @@
       <c r="R3" t="s">
         <v>13</v>
       </c>
-      <c r="S3" t="s">
-        <v>13</v>
-      </c>
-      <c r="T3" t="s">
-        <v>13</v>
-      </c>
-      <c r="U3" t="s">
-        <v>13</v>
-      </c>
-      <c r="V3" t="s">
-        <v>13</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="X3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y3" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25">
+      <c r="S3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21">
       <c r="A4" t="s">
         <v>27</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
       <c r="D4" t="s">
         <v>13</v>
       </c>
@@ -1596,6 +1564,9 @@
       <c r="F4" t="s">
         <v>13</v>
       </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
       <c r="H4" t="s">
         <v>13</v>
       </c>
@@ -1629,38 +1600,23 @@
       <c r="R4" t="s">
         <v>13</v>
       </c>
-      <c r="S4" t="s">
-        <v>13</v>
-      </c>
-      <c r="T4" t="s">
-        <v>13</v>
-      </c>
-      <c r="U4" t="s">
-        <v>13</v>
-      </c>
-      <c r="V4" t="s">
-        <v>13</v>
-      </c>
-      <c r="W4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="X4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y4" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25">
+      <c r="S4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
       <c r="A5" t="s">
         <v>29</v>
       </c>
       <c r="B5" t="s">
         <v>56</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="D5" t="s">
         <v>56</v>
       </c>
@@ -1670,6 +1626,9 @@
       <c r="F5" t="s">
         <v>56</v>
       </c>
+      <c r="G5" t="s">
+        <v>56</v>
+      </c>
       <c r="H5" t="s">
         <v>56</v>
       </c>
@@ -1703,38 +1662,23 @@
       <c r="R5" t="s">
         <v>56</v>
       </c>
-      <c r="S5" t="s">
-        <v>56</v>
-      </c>
-      <c r="T5" t="s">
-        <v>56</v>
-      </c>
-      <c r="U5" t="s">
-        <v>56</v>
-      </c>
-      <c r="V5" t="s">
-        <v>56</v>
-      </c>
-      <c r="W5" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="X5" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="Y5" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25">
+      <c r="S5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21">
       <c r="A6" t="s">
         <v>30</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="D6" s="1" t="s">
         <v>28</v>
       </c>
@@ -1744,6 +1688,9 @@
       <c r="F6" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="G6" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="H6" s="1" t="s">
         <v>28</v>
       </c>
@@ -1774,7 +1721,7 @@
       <c r="Q6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="R6" s="1" t="s">
+      <c r="R6" t="s">
         <v>28</v>
       </c>
       <c r="S6" s="1" t="s">
@@ -1786,29 +1733,14 @@
       <c r="U6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="V6" t="s">
-        <v>28</v>
-      </c>
-      <c r="W6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="X6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="Y6" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25">
+    </row>
+    <row r="7" spans="1:21">
       <c r="A7" t="s">
         <v>31</v>
       </c>
       <c r="B7" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="D7" t="s">
         <v>28</v>
       </c>
@@ -1818,6 +1750,9 @@
       <c r="F7" t="s">
         <v>28</v>
       </c>
+      <c r="G7" t="s">
+        <v>28</v>
+      </c>
       <c r="H7" t="s">
         <v>28</v>
       </c>
@@ -1851,36 +1786,21 @@
       <c r="R7" t="s">
         <v>28</v>
       </c>
-      <c r="S7" t="s">
-        <v>28</v>
-      </c>
-      <c r="T7" t="s">
-        <v>28</v>
-      </c>
-      <c r="U7" t="s">
-        <v>28</v>
-      </c>
-      <c r="V7" t="s">
-        <v>28</v>
-      </c>
-      <c r="W7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="X7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="Y7" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25">
+      <c r="S7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21">
       <c r="A8" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="B8" t="s">
         <v>28</v>
       </c>
       <c r="D8" t="s">
@@ -1892,6 +1812,9 @@
       <c r="F8" t="s">
         <v>28</v>
       </c>
+      <c r="G8" t="s">
+        <v>28</v>
+      </c>
       <c r="H8" t="s">
         <v>28</v>
       </c>
@@ -1925,38 +1848,23 @@
       <c r="R8" t="s">
         <v>28</v>
       </c>
-      <c r="S8" t="s">
-        <v>28</v>
-      </c>
-      <c r="T8" t="s">
-        <v>28</v>
-      </c>
-      <c r="U8" t="s">
-        <v>28</v>
-      </c>
-      <c r="V8" t="s">
-        <v>28</v>
-      </c>
-      <c r="W8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="X8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="Y8" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25">
+      <c r="S8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21">
       <c r="A9" t="s">
         <v>33</v>
       </c>
       <c r="B9" t="s">
         <v>56</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="D9" t="s">
         <v>56</v>
       </c>
@@ -1966,6 +1874,9 @@
       <c r="F9" t="s">
         <v>56</v>
       </c>
+      <c r="G9" t="s">
+        <v>56</v>
+      </c>
       <c r="H9" t="s">
         <v>56</v>
       </c>
@@ -1999,38 +1910,23 @@
       <c r="R9" t="s">
         <v>56</v>
       </c>
-      <c r="S9" t="s">
-        <v>56</v>
-      </c>
-      <c r="T9" t="s">
-        <v>56</v>
-      </c>
-      <c r="U9" t="s">
-        <v>56</v>
-      </c>
-      <c r="V9" t="s">
-        <v>56</v>
-      </c>
-      <c r="W9" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="X9" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="Y9" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25">
+      <c r="S9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21">
       <c r="A10" t="s">
         <v>34</v>
       </c>
       <c r="B10" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="D10" t="s">
         <v>28</v>
       </c>
@@ -2040,6 +1936,9 @@
       <c r="F10" t="s">
         <v>28</v>
       </c>
+      <c r="G10" t="s">
+        <v>28</v>
+      </c>
       <c r="H10" t="s">
         <v>28</v>
       </c>
@@ -2073,25 +1972,81 @@
       <c r="R10" t="s">
         <v>28</v>
       </c>
-      <c r="S10" t="s">
-        <v>28</v>
-      </c>
-      <c r="T10" t="s">
-        <v>28</v>
-      </c>
-      <c r="U10" t="s">
-        <v>28</v>
-      </c>
-      <c r="V10" t="s">
-        <v>28</v>
-      </c>
-      <c r="W10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="X10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="Y10" s="1" t="s">
+      <c r="S10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D418CE29-40DC-476E-89CD-A42CEC26847E}">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.5703125" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1" ht="90">
+      <c r="A2" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B5" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2100,7 +2055,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AB93"/>
   <sheetViews>
@@ -2760,7 +2715,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:P82"/>
   <sheetViews>

</xml_diff>